<commit_message>
edit gantt, wbs, AL
</commit_message>
<xml_diff>
--- a/Documentation/CSPROJ Docu/01 Gantt Chart/gantt.xlsx
+++ b/Documentation/CSPROJ Docu/01 Gantt Chart/gantt.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martha\Desktop\carkila\Documentation\CSPROJ Docu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martha\Desktop\carkila\Documentation\CSPROJ Docu\01 Gantt Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -171,13 +171,13 @@
     <t>TESTING</t>
   </si>
   <si>
-    <t>FINAL REVISION</t>
-  </si>
-  <si>
-    <t>Revise Documentation</t>
-  </si>
-  <si>
     <t>Testing/Debugging</t>
+  </si>
+  <si>
+    <t>PROJECT CLOSURE</t>
+  </si>
+  <si>
+    <t>Final Revised Documentation</t>
   </si>
 </sst>
 </file>
@@ -637,13 +637,7 @@
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -742,10 +736,10 @@
                   <c:v>Testing/Debugging</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>FINAL REVISION</c:v>
+                  <c:v>PROJECT CLOSURE</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Revise Documentation</c:v>
+                  <c:v>Final Revised Documentation</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -863,7 +857,7 @@
             <c:v>Duration</c:v>
           </c:tx>
           <c:spPr>
-            <a:gradFill flip="none" rotWithShape="1">
+            <a:gradFill>
               <a:gsLst>
                 <a:gs pos="0">
                   <a:schemeClr val="accent6">
@@ -884,18 +878,11 @@
                 </a:gs>
               </a:gsLst>
               <a:lin ang="16200000" scaled="1"/>
-              <a:tileRect/>
             </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -994,10 +981,10 @@
                   <c:v>Testing/Debugging</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>FINAL REVISION</c:v>
+                  <c:v>PROJECT CLOSURE</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Revise Documentation</c:v>
+                  <c:v>Final Revised Documentation</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1115,42 +1102,13 @@
             <c:v>Tasks</c:v>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent3">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent3">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -1249,10 +1207,10 @@
                   <c:v>Testing/Debugging</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>FINAL REVISION</c:v>
+                  <c:v>PROJECT CLOSURE</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Revise Documentation</c:v>
+                  <c:v>Final Revised Documentation</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1373,11 +1331,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="1045754864"/>
-        <c:axId val="1045758672"/>
+        <c:axId val="1037319696"/>
+        <c:axId val="1037330576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1045754864"/>
+        <c:axId val="1037319696"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1389,14 +1347,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:alpha val="54000"/>
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
-            <a:tailEnd type="triangle"/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1407,8 +1365,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1419,7 +1378,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1045758672"/>
+        <c:crossAx val="1037330576"/>
         <c:crossesAt val="42840"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1428,7 +1387,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1045758672"/>
+        <c:axId val="1037330576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42900"/>
@@ -1439,9 +1398,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1467,8 +1426,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1479,7 +1439,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1045754864"/>
+        <c:crossAx val="1037319696"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1496,28 +1456,17 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -1580,33 +1529,35 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="304">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1614,34 +1565,26 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -1650,8 +1593,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1670,6 +1614,14 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1678,20 +1630,20 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -1700,13 +1652,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="34925" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1718,10 +1670,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -1730,17 +1682,16 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -1758,18 +1709,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1788,13 +1742,14 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1806,14 +1761,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1827,8 +1782,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1842,6 +1798,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -1853,9 +1815,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1870,13 +1832,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -1888,14 +1851,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -1907,13 +1870,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -1922,13 +1886,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1936,7 +1901,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1949,21 +1914,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1971,14 +1926,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1990,19 +1945,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2018,6 +1966,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2026,8 +1975,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2043,13 +1993,14 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2058,8 +2009,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2071,6 +2023,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2376,7 +2334,7 @@
   <dimension ref="A2:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:D49"/>
+      <selection activeCell="O40" sqref="O40:P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2991,7 +2949,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C32" s="1">
         <f t="shared" si="2"/>
@@ -3011,7 +2969,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C33" s="1">
         <f>(E33-D33)</f>
@@ -3031,7 +2989,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C34" s="1">
         <f>(E34-D34)</f>

</xml_diff>